<commit_message>
improved pressure sensor code, triple working
</commit_message>
<xml_diff>
--- a/data/Calibration excell.xlsx
+++ b/data/Calibration excell.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahebe\OneDrive\Desktop\Cegep\Winter session 2022\Rocket Science\team-rocket\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\documents\école\RS\team-rocket\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BB4703-D90A-439F-A7F0-B79E0856967C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCB5863-CF2B-4B84-8DB6-833461AF7AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3F5291B0-C26C-4995-97D0-0A5A60CC0E37}"/>
+    <workbookView xWindow="10710" yWindow="1995" windowWidth="13245" windowHeight="10545" xr2:uid="{3F5291B0-C26C-4995-97D0-0A5A60CC0E37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>chiffre trouvé</t>
   </si>
@@ -49,6 +49,27 @@
   </si>
   <si>
     <t>round 2</t>
+  </si>
+  <si>
+    <t>Data from sensor's website (with 10k ohm)</t>
+  </si>
+  <si>
+    <t>poids (g)</t>
+  </si>
+  <si>
+    <t>Vout (v)</t>
+  </si>
+  <si>
+    <t>from website:</t>
+  </si>
+  <si>
+    <t>replication with extracted data:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for our measurements: </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -84,8 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +584,982 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>10kohm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.0125765529308834E-2"/>
+                  <c:y val="0.22292650918635171"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$17:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$17:$Q$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B416-413E-8B66-914C5BB80A86}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="987479039"/>
+        <c:axId val="987476543"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="987479039"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987476543"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="100"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="987476543"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="987479039"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>10kohm : useful</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.27562598425196849"/>
+                  <c:y val="5.9768518518518519E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>y = 6.7249e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="30000"/>
+                      <a:t>1.489x</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="2000" baseline="0"/>
+                      <a:t>R² = 0.9949</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="2000"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$17:$Q$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.37</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.79</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.98</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$17:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>313</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>705</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BFAB-414F-96D2-90A21D16FC58}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="731394239"/>
+        <c:axId val="731395487"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="731394239"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="731395487"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="731395487"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="731394239"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1116,6 +2115,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1149,6 +3180,128 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>247649</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>87671</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>409574</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>157820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A00BCB2B-A899-4AAE-BD7F-E1F521F8FB33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12553949" y="2373671"/>
+          <a:ext cx="4429125" cy="3308649"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5283EB08-4DB7-4096-BAFE-0ECD16D7C7C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B669E264-85CA-4E72-9F4C-F777B6C69E85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1468,19 +3621,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03AA48A8-3BC1-46AA-9D75-873D519642B5}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:V62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="T49" workbookViewId="0">
+      <selection activeCell="Q62" sqref="Q62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1488,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20</v>
       </c>
@@ -1496,7 +3649,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>59</v>
       </c>
@@ -1505,7 +3658,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>120</v>
       </c>
@@ -1514,7 +3667,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>215</v>
       </c>
@@ -1523,7 +3676,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>244</v>
       </c>
@@ -1532,7 +3685,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>245</v>
       </c>
@@ -1541,7 +3694,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>277</v>
       </c>
@@ -1550,7 +3703,7 @@
         <v>71.099999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>292</v>
       </c>
@@ -1559,7 +3712,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>300</v>
       </c>
@@ -1568,7 +3721,7 @@
         <v>80.3</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>305</v>
       </c>
@@ -1576,8 +3729,11 @@
         <f>84.1+3.6</f>
         <v>87.699999999999989</v>
       </c>
+      <c r="V12" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>567</v>
       </c>
@@ -1586,7 +3742,7 @@
         <v>202.79999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>650</v>
       </c>
@@ -1595,7 +3751,7 @@
         <v>503.6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>667</v>
       </c>
@@ -1603,8 +3759,15 @@
         <f>523.1+3.6</f>
         <v>526.70000000000005</v>
       </c>
+      <c r="O15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>755</v>
       </c>
@@ -1612,8 +3775,94 @@
         <f>1023.2+3.6</f>
         <v>1026.8</v>
       </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>22</v>
+      </c>
+      <c r="Q17">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>51</v>
+      </c>
+      <c r="Q18">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>101</v>
+      </c>
+      <c r="Q19">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>200</v>
+      </c>
+      <c r="Q20">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <v>313</v>
+      </c>
+      <c r="Q21">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>448</v>
+      </c>
+      <c r="Q22">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P23">
+        <v>565</v>
+      </c>
+      <c r="Q23">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>705</v>
+      </c>
+      <c r="Q24">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P25">
+        <v>889</v>
+      </c>
+      <c r="Q25">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>995</v>
+      </c>
+      <c r="Q26">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1624,7 +3873,25 @@
         <v>4</v>
       </c>
     </row>
+    <row r="33" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="U51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="17:21" x14ac:dyDescent="0.25">
+      <c r="Q62" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="O15:S15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">

</xml_diff>